<commit_message>
Compile official release v4.0
</commit_message>
<xml_diff>
--- a/deploy/docs/PnET-Succession function worksheet v4.0.xlsx
+++ b/deploy/docs/PnET-Succession function worksheet v4.0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egustafson\Documents\USERDOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BRM\LANDIS\GitCode\Extension-PnET-Succession\deploy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF3B1A7-A8A9-438B-9D98-CCC2B6473284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="36" windowWidth="23016" windowHeight="9096" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="-14250" yWindow="-6165" windowWidth="14400" windowHeight="14775" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PnET-Succ v. PnET-II" sheetId="9" r:id="rId1"/>
@@ -443,18 +444,27 @@
     <definedName name="WUEconst" localSheetId="0">'PnET-Succ v. PnET-II'!$AD$15</definedName>
     <definedName name="WUEconst">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Eric Gustafson</author>
   </authors>
   <commentList>
-    <comment ref="AB12" authorId="0" shapeId="0">
+    <comment ref="AB12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -483,12 +493,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Eric Gustafson</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -512,7 +522,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -536,7 +546,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -565,12 +575,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gustafson, Eric -FS</author>
   </authors>
   <commentList>
-    <comment ref="H2" authorId="0" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -599,12 +609,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gustafson, Eric -FS</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1560,7 +1570,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1939,7 +1949,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2084,6 +2094,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-688D-4FFA-BB7B-D0B07153FE63}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2193,6 +2208,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-688D-4FFA-BB7B-D0B07153FE63}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2283,7 +2303,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2449,6 +2469,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9078-4672-A8FE-1685F1B72463}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2670,7 +2695,7 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2861,6 +2886,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1742-44CD-B009-A043F3ED8889}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2979,6 +3009,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1742-44CD-B009-A043F3ED8889}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3231,7 +3266,7 @@
 </file>
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3422,6 +3457,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C59F-4592-B118-690B1DF567F2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3643,7 +3683,7 @@
 </file>
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3807,6 +3847,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6A5D-4DCF-9BD8-A003E9264F78}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3953,6 +3998,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6A5D-4DCF-9BD8-A003E9264F78}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4238,7 +4288,7 @@
 </file>
 
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4467,6 +4517,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5DD7-45C2-A23A-5F5F8F5E8DD1}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4751,7 +4806,7 @@
 </file>
 
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4970,6 +5025,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-158E-49AE-8B1F-77294F490E1E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5254,7 +5314,7 @@
 </file>
 
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5473,6 +5533,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6C45-4394-957D-0F473B0BB9AA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5619,6 +5684,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6C45-4394-957D-0F473B0BB9AA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5903,7 +5973,7 @@
 </file>
 
 <file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6097,6 +6167,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6BC5-4104-9938-847ADDB8CCC6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6381,7 +6456,7 @@
 </file>
 
 <file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6600,6 +6675,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F0A2-4841-84BE-3783905A81B2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6884,7 +6964,7 @@
 </file>
 
 <file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7063,6 +7143,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6462-48C4-92EE-573CFE044D58}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -7169,6 +7254,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6462-48C4-92EE-573CFE044D58}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -7476,7 +7566,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7621,6 +7711,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5AA8-4D28-AECE-6608D2A85468}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -7730,6 +7825,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5AA8-4D28-AECE-6608D2A85468}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -7820,7 +7920,7 @@
 </file>
 
 <file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7999,6 +8099,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF48-47C7-84F6-08E9BF47E3F4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -8105,6 +8210,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FF48-47C7-84F6-08E9BF47E3F4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -8302,7 +8412,7 @@
 </file>
 
 <file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8442,6 +8552,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2C12-48B5-99C4-A31E1456CE8C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -8509,6 +8624,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2C12-48B5-99C4-A31E1456CE8C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -8705,7 +8825,7 @@
 </file>
 
 <file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8744,7 +8864,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9011,6 +9130,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B880-4152-B5F5-862766857FC9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -9057,7 +9181,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9178,7 +9301,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9290,7 +9412,7 @@
 </file>
 
 <file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -9329,7 +9451,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9536,6 +9657,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4B9E-40E6-BBDB-B49934DDB09F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -9582,7 +9708,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9759,7 +9884,7 @@
 </file>
 
 <file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -9798,7 +9923,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9903,6 +10027,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6AE3-43B2-9B73-C2B3800B3D85}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -9949,7 +10078,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10125,7 +10253,7 @@
 </file>
 
 <file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -10430,6 +10558,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B666-4047-9870-69C7AF743ACD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -10756,7 +10889,7 @@
 </file>
 
 <file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -11050,6 +11183,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C81-481C-A365-F4D3AB63E2EE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -11271,7 +11409,7 @@
 </file>
 
 <file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -11456,6 +11594,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D9B-4B04-8F6B-C8FC486166F9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -11526,6 +11669,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2D9B-4B04-8F6B-C8FC486166F9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -11834,7 +11982,7 @@
 </file>
 
 <file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -12022,6 +12170,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-48A5-4449-B344-1E7470DD56F8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -12137,6 +12290,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-48A5-4449-B344-1E7470DD56F8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -12445,7 +12603,7 @@
 </file>
 
 <file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -12630,6 +12788,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6179-4CBC-8C7B-172A6D34A20E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -12742,6 +12905,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6179-4CBC-8C7B-172A6D34A20E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -13050,7 +13218,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -13195,6 +13363,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1CFF-41C4-9282-D35DAF292220}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -13304,6 +13477,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1CFF-41C4-9282-D35DAF292220}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -13394,7 +13572,7 @@
 </file>
 
 <file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -13554,6 +13732,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-41D2-4D9E-AF79-A355EFD1B6C8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -13831,7 +14014,7 @@
 </file>
 
 <file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -13938,6 +14121,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DEE5-47DD-888A-22B71D51CD7E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -13972,6 +14160,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DEE5-47DD-888A-22B71D51CD7E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -14278,7 +14471,7 @@
 </file>
 
 <file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -14438,6 +14631,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-70E6-4215-B8CF-17E6C313ADDA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -14659,7 +14857,7 @@
 </file>
 
 <file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -14873,6 +15071,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-93B9-4B49-8A35-E540A05C216C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -15009,6 +15212,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-93B9-4B49-8A35-E540A05C216C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -15145,6 +15353,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-93B9-4B49-8A35-E540A05C216C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -15281,6 +15494,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-93B9-4B49-8A35-E540A05C216C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -15417,6 +15635,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-93B9-4B49-8A35-E540A05C216C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -15730,7 +15953,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -15875,6 +16098,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E09D-4C3E-9E9E-BD4BBB1D273C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -15984,6 +16212,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E09D-4C3E-9E9E-BD4BBB1D273C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -16070,7 +16303,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -16215,6 +16448,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D68-4C8C-9AAE-B5EC515D86E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -16324,6 +16562,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1D68-4C8C-9AAE-B5EC515D86E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -16407,7 +16650,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -16598,6 +16841,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D5D-453C-AA22-B5CD8C68D2D6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -16716,6 +16964,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1D5D-453C-AA22-B5CD8C68D2D6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -16913,7 +17166,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -17085,6 +17338,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1381-4571-8FAE-C84860754DBF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -17179,6 +17437,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1381-4571-8FAE-C84860754DBF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -17486,7 +17749,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -17677,6 +17940,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D69A-4238-ADDB-DE974F8F2303}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -17795,6 +18063,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D69A-4238-ADDB-DE974F8F2303}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -18047,7 +18320,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -18238,6 +18511,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FCF0-4E3F-B26D-575C1FC14873}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -18356,6 +18634,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FCF0-4E3F-B26D-575C1FC14873}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -34137,7 +34420,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="图表 8"/>
+        <xdr:cNvPr id="2" name="图表 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34169,7 +34458,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="图表 16"/>
+        <xdr:cNvPr id="3" name="图表 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34201,7 +34496,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="图表 17"/>
+        <xdr:cNvPr id="4" name="图表 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34233,7 +34534,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="图表 18"/>
+        <xdr:cNvPr id="5" name="图表 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34265,7 +34572,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="图表 1"/>
+        <xdr:cNvPr id="6" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34297,7 +34610,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34334,7 +34653,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34369,7 +34694,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34401,7 +34732,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34433,7 +34770,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34470,7 +34813,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34505,7 +34854,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34535,7 +34890,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34570,7 +34931,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34601,7 +34968,13 @@
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="3" name="Straight Connector 2"/>
+        <cdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54CF450A-9058-46F9-B9DC-E1DF30DC6233}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
@@ -34649,7 +35022,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34684,7 +35063,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34714,7 +35099,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34746,7 +35137,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34778,7 +35175,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34810,7 +35213,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -34845,7 +35254,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34877,7 +35292,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34909,7 +35330,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34941,7 +35368,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -34973,7 +35406,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -35003,7 +35442,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -35038,7 +35483,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -35068,7 +35519,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -35098,7 +35555,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -35133,7 +35596,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -35163,7 +35632,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -35193,7 +35668,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -35224,7 +35705,13 @@
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="3" name="Straight Connector 2"/>
+        <cdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6D8FA5C-2664-4335-B7A6-B14B54C78EF8}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
@@ -35268,7 +35755,13 @@
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="2" name="Straight Connector 1"/>
+        <cdr:cNvPr id="2" name="Straight Connector 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D2619EC-29C4-4A12-94AA-EC59B18BC29C}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
@@ -35316,7 +35809,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -35412,6 +35911,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -35447,6 +35963,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -35622,7 +36155,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BE77"/>
   <sheetViews>
@@ -35630,40 +36163,40 @@
       <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="6" width="9.109375" style="24"/>
+    <col min="1" max="6" width="9.08984375" style="24"/>
     <col min="7" max="8" width="0" style="24" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="24"/>
-    <col min="10" max="10" width="14.44140625" style="24" customWidth="1"/>
+    <col min="9" max="9" width="9.08984375" style="24"/>
+    <col min="10" max="10" width="14.453125" style="24" customWidth="1"/>
     <col min="11" max="11" width="15" style="24" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" style="24" customWidth="1"/>
-    <col min="13" max="13" width="19.44140625" style="24" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" style="24" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" style="24" customWidth="1"/>
-    <col min="16" max="16" width="19.109375" style="24" customWidth="1"/>
-    <col min="17" max="17" width="13.44140625" style="24" customWidth="1"/>
-    <col min="18" max="18" width="19.109375" style="24" customWidth="1"/>
-    <col min="19" max="20" width="13.6640625" style="24" customWidth="1"/>
-    <col min="21" max="21" width="21.6640625" style="24" customWidth="1"/>
-    <col min="22" max="22" width="15.33203125" style="24" customWidth="1"/>
-    <col min="23" max="23" width="19.44140625" style="24" customWidth="1"/>
-    <col min="24" max="24" width="21.44140625" style="24" customWidth="1"/>
-    <col min="25" max="25" width="23.33203125" style="24" customWidth="1"/>
-    <col min="26" max="26" width="20.5546875" style="24" customWidth="1"/>
+    <col min="12" max="12" width="15.08984375" style="24" customWidth="1"/>
+    <col min="13" max="13" width="19.453125" style="24" customWidth="1"/>
+    <col min="14" max="14" width="19.6328125" style="24" customWidth="1"/>
+    <col min="15" max="15" width="21.6328125" style="24" customWidth="1"/>
+    <col min="16" max="16" width="19.08984375" style="24" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" style="24" customWidth="1"/>
+    <col min="18" max="18" width="19.08984375" style="24" customWidth="1"/>
+    <col min="19" max="20" width="13.6328125" style="24" customWidth="1"/>
+    <col min="21" max="21" width="21.6328125" style="24" customWidth="1"/>
+    <col min="22" max="22" width="15.36328125" style="24" customWidth="1"/>
+    <col min="23" max="23" width="19.453125" style="24" customWidth="1"/>
+    <col min="24" max="24" width="21.453125" style="24" customWidth="1"/>
+    <col min="25" max="25" width="23.36328125" style="24" customWidth="1"/>
+    <col min="26" max="26" width="20.54296875" style="24" customWidth="1"/>
     <col min="27" max="27" width="7" style="24" customWidth="1"/>
-    <col min="28" max="28" width="14.88671875" style="24" customWidth="1"/>
-    <col min="29" max="30" width="9.109375" style="24"/>
-    <col min="31" max="31" width="13.6640625" style="24" customWidth="1"/>
-    <col min="32" max="32" width="9.109375" style="24"/>
-    <col min="33" max="33" width="14.109375" style="24" customWidth="1"/>
-    <col min="34" max="34" width="10.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.109375" style="24"/>
-    <col min="36" max="36" width="16.33203125" style="24" customWidth="1"/>
-    <col min="37" max="37" width="16.88671875" style="24" customWidth="1"/>
-    <col min="38" max="43" width="9.109375" style="24"/>
-    <col min="44" max="44" width="11.6640625" style="24" customWidth="1"/>
-    <col min="45" max="16384" width="9.109375" style="24"/>
+    <col min="28" max="28" width="14.90625" style="24" customWidth="1"/>
+    <col min="29" max="30" width="9.08984375" style="24"/>
+    <col min="31" max="31" width="13.6328125" style="24" customWidth="1"/>
+    <col min="32" max="32" width="9.08984375" style="24"/>
+    <col min="33" max="33" width="14.08984375" style="24" customWidth="1"/>
+    <col min="34" max="34" width="10.36328125" style="24" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.08984375" style="24"/>
+    <col min="36" max="36" width="16.36328125" style="24" customWidth="1"/>
+    <col min="37" max="37" width="16.90625" style="24" customWidth="1"/>
+    <col min="38" max="43" width="9.08984375" style="24"/>
+    <col min="44" max="44" width="11.6328125" style="24" customWidth="1"/>
+    <col min="45" max="16384" width="9.08984375" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57" ht="15" thickBot="1">
@@ -38942,23 +39475,23 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="24"/>
-    <col min="2" max="2" width="9.109375" style="24" customWidth="1"/>
-    <col min="3" max="4" width="9.109375" style="24" hidden="1" customWidth="1"/>
-    <col min="5" max="11" width="9.109375" style="24"/>
+    <col min="1" max="1" width="9.08984375" style="24"/>
+    <col min="2" max="2" width="9.08984375" style="24" customWidth="1"/>
+    <col min="3" max="4" width="9.08984375" style="24" hidden="1" customWidth="1"/>
+    <col min="5" max="11" width="9.08984375" style="24"/>
     <col min="12" max="12" width="16" style="24" customWidth="1"/>
-    <col min="13" max="16" width="9.109375" style="24"/>
+    <col min="13" max="16" width="9.08984375" style="24"/>
     <col min="17" max="17" width="12" style="24" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="24"/>
+    <col min="18" max="16384" width="9.08984375" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -40057,7 +40590,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:O33"/>
   <sheetViews>
@@ -40065,11 +40598,11 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="5" max="5" width="10.21875" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="24"/>
-    <col min="12" max="12" width="8.88671875" style="24"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" style="24"/>
+    <col min="12" max="12" width="8.90625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="24" customFormat="1">
@@ -40525,7 +41058,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -40533,17 +41066,17 @@
       <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="24"/>
-    <col min="2" max="2" width="10.109375" style="24" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="24" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="24" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="24" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" style="24" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="24"/>
+    <col min="1" max="1" width="9.08984375" style="24"/>
+    <col min="2" max="2" width="10.08984375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="6.54296875" style="24" customWidth="1"/>
+    <col min="9" max="16384" width="9.08984375" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -40809,7 +41342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:P22"/>
   <sheetViews>
@@ -40817,11 +41350,11 @@
       <selection activeCell="I5" sqref="I5:K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13" style="24" customWidth="1"/>
     <col min="2" max="2" width="7" style="24" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="24"/>
+    <col min="3" max="16384" width="9.08984375" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -41404,7 +41937,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -41412,7 +41945,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -41592,7 +42125,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AD20"/>
   <sheetViews>
@@ -41600,15 +42133,15 @@
       <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="24"/>
-    <col min="12" max="12" width="9.109375" style="24"/>
-    <col min="15" max="15" width="9.109375" style="24"/>
-    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.88671875" customWidth="1"/>
-    <col min="27" max="27" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.08984375" style="24"/>
+    <col min="12" max="12" width="9.08984375" style="24"/>
+    <col min="15" max="15" width="9.08984375" style="24"/>
+    <col min="19" max="19" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.90625" customWidth="1"/>
+    <col min="27" max="27" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -43099,7 +43632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Y32"/>
   <sheetViews>
@@ -43107,14 +43640,14 @@
       <selection activeCell="S15" sqref="S15:S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="8" max="8" width="9.109375" style="24"/>
-    <col min="9" max="17" width="9.109375" style="4"/>
-    <col min="18" max="18" width="12.5546875" customWidth="1"/>
-    <col min="22" max="22" width="9.109375" style="4"/>
-    <col min="25" max="25" width="10.44140625" style="4" customWidth="1"/>
-    <col min="27" max="27" width="8.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.08984375" style="24"/>
+    <col min="9" max="17" width="9.08984375" style="4"/>
+    <col min="18" max="18" width="12.54296875" customWidth="1"/>
+    <col min="22" max="22" width="9.08984375" style="4"/>
+    <col min="25" max="25" width="10.453125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="8.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -44381,7 +44914,7 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1" display="A@ref"/>
+    <hyperlink ref="E1" r:id="rId1" display="A@ref" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -44391,7 +44924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:M19"/>
   <sheetViews>
@@ -44399,18 +44932,18 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="24"/>
-    <col min="3" max="3" width="10.33203125" style="24" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" style="24"/>
+    <col min="3" max="3" width="10.36328125" style="24" customWidth="1"/>
     <col min="4" max="4" width="11" style="24" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="24" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="24" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="24"/>
-    <col min="9" max="9" width="10.109375" style="24" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="24"/>
+    <col min="5" max="5" width="11.54296875" style="24" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="9.08984375" style="24"/>
+    <col min="9" max="9" width="10.08984375" style="24" customWidth="1"/>
+    <col min="10" max="16384" width="9.08984375" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -45052,19 +45585,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -45230,18 +45763,18 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G20" sqref="G20:H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" customWidth="1"/>
     <col min="22" max="22" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -45899,7 +46432,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Y3" r:id="rId1"/>
+    <hyperlink ref="Y3" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -45907,7 +46440,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:J32"/>
   <sheetViews>
@@ -45915,14 +46448,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="24"/>
-    <col min="2" max="2" width="12.44140625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="24"/>
-    <col min="5" max="5" width="14.21875" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="24"/>
+    <col min="1" max="1" width="9.08984375" style="24"/>
+    <col min="2" max="2" width="12.453125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="9.08984375" style="24"/>
+    <col min="5" max="5" width="14.1796875" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="9.08984375" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -45979,7 +46512,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.6">
+    <row r="4" spans="1:10" ht="15.5">
       <c r="A4" s="24">
         <v>20</v>
       </c>
@@ -46269,7 +46802,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -46277,9 +46810,9 @@
       <selection activeCell="G1" sqref="G1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -46338,7 +46871,7 @@
         <v>0.89047522329747264</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6">
+    <row r="5" spans="1:9" ht="15.5">
       <c r="A5" s="24">
         <f t="shared" si="0"/>
         <v>4300</v>

</xml_diff>

<commit_message>
Update layering and sublayer shuffling each timestep within spinup. Do not allow nsc to be negative.
</commit_message>
<xml_diff>
--- a/deploy/docs/PnET-Succession function worksheet v4.0.xlsx
+++ b/deploy/docs/PnET-Succession function worksheet v4.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BRM\LANDIS\GitCode\Extension-PnET-Succession\deploy\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BRM\LANDIS_II\GitCode\Extension-PnET-Succession\deploy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF3B1A7-A8A9-438B-9D98-CCC2B6473284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7137A9C2-E7DC-4C0C-AF6C-6925F41B8192}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14250" yWindow="-6165" windowWidth="14400" windowHeight="14775" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PnET-Succ v. PnET-II" sheetId="9" r:id="rId1"/>
@@ -643,7 +643,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="310">
   <si>
     <t>Shape parameter</t>
   </si>
@@ -1566,6 +1566,24 @@
   <si>
     <t>fWater calculator</t>
   </si>
+  <si>
+    <t>PAR</t>
+  </si>
+  <si>
+    <t>fRad1</t>
+  </si>
+  <si>
+    <t>fRad2</t>
+  </si>
+  <si>
+    <t>HalfSat1</t>
+  </si>
+  <si>
+    <t>HalfSat2</t>
+  </si>
+  <si>
+    <t>Compare two fRad curves with different HalfSat values</t>
+  </si>
 </sst>
 </file>
 
@@ -8838,6 +8856,728 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fRad!$B$13:$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>HalfSat1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fRad!$A$16:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fRad!$B$16:$B$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.90909090909090906</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90476190476190477</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89473684210526316</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.88235294117647056</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8571428571428571</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84615384615384615</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.83333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.81818181818181823</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.77777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.7142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8D68-4CA8-B00C-BF7F00DD1950}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fRad!$C$13:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>HalfSat2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fRad!$A$16:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fRad!$C$16:$C$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.76923076923076927</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.73913043478260865</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72727272727272729</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68421052631578949</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6470588235294118</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.53846153846153844</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.45454545454545453</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.14285714285714285</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8D68-4CA8-B00C-BF7F00DD1950}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1777265536"/>
+        <c:axId val="1928178048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1777265536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PAR</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1928178048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1928178048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>fRad</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1777265536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.64316601049868771"/>
+          <c:y val="0.50983741615631384"/>
+          <c:w val="0.21238954505686788"/>
+          <c:h val="0.15625109361329836"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
@@ -9411,7 +10151,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -9883,7 +10623,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -10252,7 +10992,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -10888,7 +11628,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -11408,7 +12148,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -11981,7 +12721,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -12602,7 +13342,361 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Layer Foliar Respiration</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'PnET-Succ v. PnET-II'!$V$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FolResp[layer]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'PnET-Succ v. PnET-II'!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'PnET-Succ v. PnET-II'!$V$2:$V$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.1392320960222382</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6111174808853779</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2784641920444764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2222349617707553</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5569283840889527</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4444699235415106</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.1138567681779055</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.888939847083021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.227713536355811</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.777879694166042</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36.455427072711622</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>51.555759388332085</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1CFF-41C4-9282-D35DAF292220}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'PnET-Succ v. PnET-II'!$V$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LayerResp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'PnET-Succ v. PnET-II'!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'PnET-Succ v. PnET-II'!$V$21:$V$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.2083381106640332</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7088481440333574</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4166762213280659</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4176962880667152</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8333524426561318</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8353925761334304</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.6667048853122637</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.670785152266861</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.333409770624527</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.341570304533718</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38.666819541249055</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54.683140609067422</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1CFF-41C4-9282-D35DAF292220}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="597984712"/>
+        <c:axId val="597978832"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="597984712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="597978832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="597978832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>gC/layer/mo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="597984712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -13217,361 +14311,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Layer Foliar Respiration</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'PnET-Succ v. PnET-II'!$V$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>FolResp[layer]</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'PnET-Succ v. PnET-II'!$E$2:$E$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'PnET-Succ v. PnET-II'!$V$2:$V$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>1.1392320960222382</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.6111174808853779</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.2784641920444764</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.2222349617707553</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.5569283840889527</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.4444699235415106</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.1138567681779055</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12.888939847083021</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18.227713536355811</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>25.777879694166042</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>36.455427072711622</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>51.555759388332085</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1CFF-41C4-9282-D35DAF292220}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'PnET-Succ v. PnET-II'!$V$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>LayerResp</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'PnET-Succ v. PnET-II'!$E$2:$E$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'PnET-Succ v. PnET-II'!$V$21:$V$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>1.2083381106640332</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7088481440333574</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.4166762213280659</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.4176962880667152</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.8333524426561318</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.8353925761334304</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.6667048853122637</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13.670785152266861</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>19.333409770624527</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>27.341570304533718</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>38.666819541249055</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>54.683140609067422</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1CFF-41C4-9282-D35DAF292220}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="597984712"/>
-        <c:axId val="597978832"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="597984712"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="597978832"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="597978832"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>gC/layer/mo</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
-                  <a:t> </a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="597984712"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -14013,7 +14753,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -14470,7 +15210,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -14856,7 +15596,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -19675,6 +20415,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors29.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -24084,7 +24864,7 @@
 </file>
 
 <file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -24111,8 +24891,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -24192,11 +24972,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -24207,11 +24982,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -24223,7 +24993,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -24243,9 +25013,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -24258,10 +25025,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -24301,22 +25068,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -24421,8 +25189,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -24554,19 +25322,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -24580,6 +25349,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -30276,6 +31056,522 @@
 </file>
 
 <file path=xl/charts/style28.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style29.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -34641,6 +35937,49 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
@@ -34677,7 +36016,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -34796,7 +36135,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -34837,7 +36176,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -34914,7 +36253,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -34955,7 +36294,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -35584,6 +36923,47 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA77D3C2-5A7F-4EF6-9A25-F765B1B24530}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -35692,7 +37072,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -35742,7 +37122,7 @@
 </c:userShapes>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -35790,49 +37170,6 @@
     </cdr:cxnSp>
   </cdr:relSizeAnchor>
 </c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36163,43 +37500,43 @@
       <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="6" width="9.08984375" style="24"/>
+    <col min="1" max="6" width="9.140625" style="24"/>
     <col min="7" max="8" width="0" style="24" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.08984375" style="24"/>
-    <col min="10" max="10" width="14.453125" style="24" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="24"/>
+    <col min="10" max="10" width="14.42578125" style="24" customWidth="1"/>
     <col min="11" max="11" width="15" style="24" customWidth="1"/>
-    <col min="12" max="12" width="15.08984375" style="24" customWidth="1"/>
-    <col min="13" max="13" width="19.453125" style="24" customWidth="1"/>
-    <col min="14" max="14" width="19.6328125" style="24" customWidth="1"/>
-    <col min="15" max="15" width="21.6328125" style="24" customWidth="1"/>
-    <col min="16" max="16" width="19.08984375" style="24" customWidth="1"/>
-    <col min="17" max="17" width="13.453125" style="24" customWidth="1"/>
-    <col min="18" max="18" width="19.08984375" style="24" customWidth="1"/>
-    <col min="19" max="20" width="13.6328125" style="24" customWidth="1"/>
-    <col min="21" max="21" width="21.6328125" style="24" customWidth="1"/>
-    <col min="22" max="22" width="15.36328125" style="24" customWidth="1"/>
-    <col min="23" max="23" width="19.453125" style="24" customWidth="1"/>
-    <col min="24" max="24" width="21.453125" style="24" customWidth="1"/>
-    <col min="25" max="25" width="23.36328125" style="24" customWidth="1"/>
-    <col min="26" max="26" width="20.54296875" style="24" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="24" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" style="24" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" style="24" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" style="24" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" style="24" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" style="24" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" style="24" customWidth="1"/>
+    <col min="19" max="20" width="13.5703125" style="24" customWidth="1"/>
+    <col min="21" max="21" width="21.5703125" style="24" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="24" customWidth="1"/>
+    <col min="23" max="23" width="19.42578125" style="24" customWidth="1"/>
+    <col min="24" max="24" width="21.42578125" style="24" customWidth="1"/>
+    <col min="25" max="25" width="23.42578125" style="24" customWidth="1"/>
+    <col min="26" max="26" width="20.5703125" style="24" customWidth="1"/>
     <col min="27" max="27" width="7" style="24" customWidth="1"/>
-    <col min="28" max="28" width="14.90625" style="24" customWidth="1"/>
-    <col min="29" max="30" width="9.08984375" style="24"/>
-    <col min="31" max="31" width="13.6328125" style="24" customWidth="1"/>
-    <col min="32" max="32" width="9.08984375" style="24"/>
-    <col min="33" max="33" width="14.08984375" style="24" customWidth="1"/>
-    <col min="34" max="34" width="10.36328125" style="24" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.08984375" style="24"/>
-    <col min="36" max="36" width="16.36328125" style="24" customWidth="1"/>
-    <col min="37" max="37" width="16.90625" style="24" customWidth="1"/>
-    <col min="38" max="43" width="9.08984375" style="24"/>
-    <col min="44" max="44" width="11.6328125" style="24" customWidth="1"/>
-    <col min="45" max="16384" width="9.08984375" style="24"/>
+    <col min="28" max="28" width="14.85546875" style="24" customWidth="1"/>
+    <col min="29" max="30" width="9.140625" style="24"/>
+    <col min="31" max="31" width="13.5703125" style="24" customWidth="1"/>
+    <col min="32" max="32" width="9.140625" style="24"/>
+    <col min="33" max="33" width="14.140625" style="24" customWidth="1"/>
+    <col min="34" max="34" width="10.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.140625" style="24"/>
+    <col min="36" max="36" width="16.42578125" style="24" customWidth="1"/>
+    <col min="37" max="37" width="16.85546875" style="24" customWidth="1"/>
+    <col min="38" max="43" width="9.140625" style="24"/>
+    <col min="44" max="44" width="11.5703125" style="24" customWidth="1"/>
+    <col min="45" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="15" thickBot="1">
+    <row r="1" spans="1:57" ht="15.75" thickBot="1">
       <c r="A1" s="24" t="s">
         <v>57</v>
       </c>
@@ -37446,7 +38783,7 @@
       <c r="AH12" s="43"/>
       <c r="AI12" s="43"/>
     </row>
-    <row r="13" spans="1:57" ht="15" thickBot="1">
+    <row r="13" spans="1:57" ht="15.75" thickBot="1">
       <c r="B13" s="24">
         <v>40</v>
       </c>
@@ -37669,7 +39006,7 @@
       </c>
       <c r="AE18" s="4"/>
     </row>
-    <row r="19" spans="1:49" ht="15" thickBot="1">
+    <row r="19" spans="1:49" ht="15.75" thickBot="1">
       <c r="G19" s="24" t="s">
         <v>105</v>
       </c>
@@ -37708,7 +39045,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:49" ht="15" thickBot="1">
+    <row r="20" spans="1:49" ht="15.75" thickBot="1">
       <c r="A20" s="24" t="s">
         <v>54</v>
       </c>
@@ -37786,7 +39123,7 @@
       <c r="AV20" s="8"/>
       <c r="AW20" s="8"/>
     </row>
-    <row r="21" spans="1:49" ht="15" thickBot="1">
+    <row r="21" spans="1:49" ht="15.75" thickBot="1">
       <c r="G21" s="11">
         <f>IF(Tday &lt;0,0.61078 * EXP(21.87456 * Tday / (Tday + 265.5)),0.61078 * EXP(17.26939 * Tday / (Tday + 237.3)))</f>
         <v>0.61077999999999999</v>
@@ -37880,7 +39217,7 @@
       <c r="AV21" s="8"/>
       <c r="AW21" s="8"/>
     </row>
-    <row r="22" spans="1:49" ht="15" thickBot="1">
+    <row r="22" spans="1:49" ht="15.75" thickBot="1">
       <c r="G22" s="11">
         <f>IF(E3 &lt;0,0.61078 * EXP(21.87456 * E3 / (E3 + 265.5)),0.61078 * EXP(17.26939 * E3 / (E3 + 237.3)))</f>
         <v>0.87227141748882542</v>
@@ -37965,7 +39302,7 @@
       <c r="AV22" s="8"/>
       <c r="AW22" s="8"/>
     </row>
-    <row r="23" spans="1:49" ht="15" thickBot="1">
+    <row r="23" spans="1:49" ht="15.75" thickBot="1">
       <c r="G23" s="11">
         <f t="shared" ref="G23:G32" si="31">IF(E4 &lt;0,0.61078 * EXP(21.87456 * E4 / (E4 + 265.5)),0.61078 * EXP(17.26939 * E4 / (E4 + 237.3)))</f>
         <v>1.2278921229539039</v>
@@ -38051,7 +39388,7 @@
       <c r="AV23" s="8"/>
       <c r="AW23" s="8"/>
     </row>
-    <row r="24" spans="1:49" ht="15" thickBot="1">
+    <row r="24" spans="1:49" ht="15.75" thickBot="1">
       <c r="G24" s="11">
         <f t="shared" si="31"/>
         <v>1.7052285488209411</v>
@@ -38140,7 +39477,7 @@
       <c r="AV24" s="8"/>
       <c r="AW24" s="8"/>
     </row>
-    <row r="25" spans="1:49" ht="15" thickBot="1">
+    <row r="25" spans="1:49" ht="15.75" thickBot="1">
       <c r="G25" s="11">
         <f t="shared" si="31"/>
         <v>2.3380938419374377</v>
@@ -38233,7 +39570,7 @@
       <c r="AV25" s="8"/>
       <c r="AW25" s="8"/>
     </row>
-    <row r="26" spans="1:49" ht="15" thickBot="1">
+    <row r="26" spans="1:49" ht="15.75" thickBot="1">
       <c r="G26" s="11">
         <f t="shared" si="31"/>
         <v>3.1674898302368564</v>
@@ -38325,7 +39662,7 @@
       <c r="AV26" s="8"/>
       <c r="AW26" s="8"/>
     </row>
-    <row r="27" spans="1:49" ht="15" thickBot="1">
+    <row r="27" spans="1:49" ht="15.75" thickBot="1">
       <c r="G27" s="11">
         <f t="shared" si="31"/>
         <v>4.2426356531114431</v>
@@ -38409,7 +39746,7 @@
       <c r="AV27" s="8"/>
       <c r="AW27" s="8"/>
     </row>
-    <row r="28" spans="1:49" ht="15" thickBot="1">
+    <row r="28" spans="1:49" ht="15.75" thickBot="1">
       <c r="G28" s="11">
         <f t="shared" si="31"/>
         <v>5.6220563085635584</v>
@@ -38493,7 +39830,7 @@
       <c r="AV28" s="8"/>
       <c r="AW28" s="8"/>
     </row>
-    <row r="29" spans="1:49" ht="15" thickBot="1">
+    <row r="29" spans="1:49" ht="15.75" thickBot="1">
       <c r="G29" s="11">
         <f t="shared" si="31"/>
         <v>7.3747231460360023</v>
@@ -38579,7 +39916,7 @@
       <c r="AV29" s="8"/>
       <c r="AW29" s="8"/>
     </row>
-    <row r="30" spans="1:49" ht="15" thickBot="1">
+    <row r="30" spans="1:49" ht="15.75" thickBot="1">
       <c r="G30" s="11">
         <f t="shared" si="31"/>
         <v>9.5812372781996284</v>
@@ -38675,7 +40012,7 @@
       <c r="AV30" s="8"/>
       <c r="AW30" s="8"/>
     </row>
-    <row r="31" spans="1:49" ht="15" thickBot="1">
+    <row r="31" spans="1:49" ht="15.75" thickBot="1">
       <c r="G31" s="11">
         <f t="shared" si="31"/>
         <v>12.335046017492973</v>
@@ -38764,7 +40101,7 @@
       <c r="AV31" s="8"/>
       <c r="AW31" s="8"/>
     </row>
-    <row r="32" spans="1:49" ht="15" thickBot="1">
+    <row r="32" spans="1:49" ht="15.75" thickBot="1">
       <c r="G32" s="12">
         <f t="shared" si="31"/>
         <v>15.743681776119971</v>
@@ -38850,7 +40187,7 @@
       <c r="AV32" s="8"/>
       <c r="AW32" s="8"/>
     </row>
-    <row r="33" spans="1:49" ht="15" thickBot="1">
+    <row r="33" spans="1:49" ht="15.75" thickBot="1">
       <c r="A33" s="48" t="s">
         <v>175</v>
       </c>
@@ -39482,16 +40819,16 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="24"/>
-    <col min="2" max="2" width="9.08984375" style="24" customWidth="1"/>
-    <col min="3" max="4" width="9.08984375" style="24" hidden="1" customWidth="1"/>
-    <col min="5" max="11" width="9.08984375" style="24"/>
+    <col min="1" max="1" width="9.140625" style="24"/>
+    <col min="2" max="2" width="9.140625" style="24" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="24" hidden="1" customWidth="1"/>
+    <col min="5" max="11" width="9.140625" style="24"/>
     <col min="12" max="12" width="16" style="24" customWidth="1"/>
-    <col min="13" max="16" width="9.08984375" style="24"/>
+    <col min="13" max="16" width="9.140625" style="24"/>
     <col min="17" max="17" width="12" style="24" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.08984375" style="24"/>
+    <col min="18" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -40598,11 +41935,11 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" style="24"/>
-    <col min="12" max="12" width="8.90625" style="24"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="24"/>
+    <col min="12" max="12" width="8.85546875" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="24" customFormat="1">
@@ -41066,17 +42403,17 @@
       <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="24"/>
-    <col min="2" max="2" width="10.08984375" style="24" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="24" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="24" customWidth="1"/>
-    <col min="6" max="6" width="9.90625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="11.36328125" style="24" customWidth="1"/>
-    <col min="8" max="8" width="6.54296875" style="24" customWidth="1"/>
-    <col min="9" max="16384" width="9.08984375" style="24"/>
+    <col min="1" max="1" width="9.140625" style="24"/>
+    <col min="2" max="2" width="10.140625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="24" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="24" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -41350,11 +42687,11 @@
       <selection activeCell="I5" sqref="I5:K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" style="24" customWidth="1"/>
     <col min="2" max="2" width="7" style="24" customWidth="1"/>
-    <col min="3" max="16384" width="9.08984375" style="24"/>
+    <col min="3" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -41945,7 +43282,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -42133,15 +43470,15 @@
       <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="9.08984375" style="24"/>
-    <col min="12" max="12" width="9.08984375" style="24"/>
-    <col min="15" max="15" width="9.08984375" style="24"/>
-    <col min="19" max="19" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.90625" customWidth="1"/>
-    <col min="27" max="27" width="11.6328125" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="24"/>
+    <col min="12" max="12" width="9.140625" style="24"/>
+    <col min="15" max="15" width="9.140625" style="24"/>
+    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.85546875" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -43640,14 +44977,14 @@
       <selection activeCell="S15" sqref="S15:S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="9.08984375" style="24"/>
-    <col min="9" max="17" width="9.08984375" style="4"/>
-    <col min="18" max="18" width="12.54296875" customWidth="1"/>
-    <col min="22" max="22" width="9.08984375" style="4"/>
-    <col min="25" max="25" width="10.453125" style="4" customWidth="1"/>
-    <col min="27" max="27" width="8.08984375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="24"/>
+    <col min="9" max="17" width="9.140625" style="4"/>
+    <col min="18" max="18" width="12.5703125" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="4"/>
+    <col min="25" max="25" width="10.42578125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -44932,18 +46269,18 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" style="24"/>
-    <col min="3" max="3" width="10.36328125" style="24" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="24"/>
+    <col min="3" max="3" width="10.42578125" style="24" customWidth="1"/>
     <col min="4" max="4" width="11" style="24" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" style="24" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="24" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" style="24" customWidth="1"/>
-    <col min="8" max="8" width="9.08984375" style="24"/>
-    <col min="9" max="9" width="10.08984375" style="24" customWidth="1"/>
-    <col min="10" max="16384" width="9.08984375" style="24"/>
+    <col min="5" max="5" width="11.5703125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="24"/>
+    <col min="9" max="9" width="10.140625" style="24" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -45586,18 +46923,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16:K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -45755,10 +47092,348 @@
       <c r="B11" s="24"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="B12" s="24"/>
+      <c r="A12" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="B13" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="B14" s="28">
+        <v>100</v>
+      </c>
+      <c r="C14" s="28">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="B15" t="s">
+        <v>305</v>
+      </c>
+      <c r="C15" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="24">
+        <v>1000</v>
+      </c>
+      <c r="B16" s="26">
+        <f>$A16/($A16+B$14)</f>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="C16" s="26">
+        <f>$A16/($A16+C$14)</f>
+        <v>0.76923076923076927</v>
+      </c>
+      <c r="K16">
+        <f>(-B$14*B16)/(B16-1)</f>
+        <v>999.99999999999966</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="24">
+        <v>950</v>
+      </c>
+      <c r="B17" s="26">
+        <f t="shared" ref="B17:C36" si="0">$A17/($A17+B$14)</f>
+        <v>0.90476190476190477</v>
+      </c>
+      <c r="C17" s="26">
+        <f t="shared" si="0"/>
+        <v>0.76</v>
+      </c>
+      <c r="K17" s="24">
+        <f t="shared" ref="K17:K23" si="1">(-B$14*B17)/(B17-1)</f>
+        <v>950.00000000000011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="24">
+        <v>900</v>
+      </c>
+      <c r="B18" s="26">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="C18" s="26">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="K18" s="24">
+        <f t="shared" si="1"/>
+        <v>900.00000000000023</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="24">
+        <v>850</v>
+      </c>
+      <c r="B19" s="26">
+        <f t="shared" si="0"/>
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="C19" s="26">
+        <f t="shared" si="0"/>
+        <v>0.73913043478260865</v>
+      </c>
+      <c r="K19" s="24">
+        <f t="shared" si="1"/>
+        <v>850</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="24">
+        <v>800</v>
+      </c>
+      <c r="B20" s="26">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="C20" s="26">
+        <f t="shared" si="0"/>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="K20" s="24">
+        <f t="shared" si="1"/>
+        <v>799.99999999999966</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="24">
+        <v>750</v>
+      </c>
+      <c r="B21" s="26">
+        <f t="shared" si="0"/>
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="C21" s="26">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="K21" s="24">
+        <f t="shared" si="1"/>
+        <v>749.99999999999977</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="24">
+        <v>700</v>
+      </c>
+      <c r="B22" s="26">
+        <f t="shared" si="0"/>
+        <v>0.875</v>
+      </c>
+      <c r="C22" s="26">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="K22" s="24">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="24">
+        <v>650</v>
+      </c>
+      <c r="B23" s="26">
+        <f t="shared" si="0"/>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="C23" s="26">
+        <f t="shared" si="0"/>
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="K23" s="24">
+        <f t="shared" si="1"/>
+        <v>650.00000000000023</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="24">
+        <v>600</v>
+      </c>
+      <c r="B24" s="26">
+        <f t="shared" si="0"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="C24" s="26">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="24">
+        <v>550</v>
+      </c>
+      <c r="B25" s="26">
+        <f t="shared" si="0"/>
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="C25" s="26">
+        <f t="shared" si="0"/>
+        <v>0.6470588235294118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="24">
+        <v>500</v>
+      </c>
+      <c r="B26" s="26">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C26" s="26">
+        <f t="shared" si="0"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="24">
+        <v>450</v>
+      </c>
+      <c r="B27" s="26">
+        <f t="shared" si="0"/>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="C27" s="26">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="24">
+        <v>400</v>
+      </c>
+      <c r="B28" s="26">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="C28" s="26">
+        <f t="shared" si="0"/>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="24">
+        <v>350</v>
+      </c>
+      <c r="B29" s="26">
+        <f t="shared" si="0"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="C29" s="26">
+        <f t="shared" si="0"/>
+        <v>0.53846153846153844</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="24">
+        <v>300</v>
+      </c>
+      <c r="B30" s="26">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="C30" s="26">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="24">
+        <v>250</v>
+      </c>
+      <c r="B31" s="26">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="C31" s="26">
+        <f t="shared" si="0"/>
+        <v>0.45454545454545453</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="24">
+        <v>200</v>
+      </c>
+      <c r="B32" s="26">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C32" s="26">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="24">
+        <v>150</v>
+      </c>
+      <c r="B33" s="26">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="C33" s="26">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="24">
+        <v>100</v>
+      </c>
+      <c r="B34" s="26">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C34" s="26">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="24">
+        <v>50</v>
+      </c>
+      <c r="B35" s="26">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C35" s="26">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="24">
+        <v>0</v>
+      </c>
+      <c r="B36" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C36" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -45767,14 +47442,14 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G20" sqref="G20:H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
     <col min="22" max="22" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -46448,14 +48123,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="24"/>
-    <col min="2" max="2" width="12.453125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="9.08984375" style="24"/>
-    <col min="5" max="5" width="14.1796875" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="9.08984375" style="24"/>
+    <col min="1" max="1" width="9.140625" style="24"/>
+    <col min="2" max="2" width="12.42578125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="24"/>
+    <col min="5" max="5" width="14.140625" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -46512,7 +48187,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.5">
+    <row r="4" spans="1:10" ht="15.75">
       <c r="A4" s="24">
         <v>20</v>
       </c>
@@ -46810,9 +48485,9 @@
       <selection activeCell="G1" sqref="G1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -46871,7 +48546,7 @@
         <v>0.89047522329747264</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.5">
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="24">
         <f t="shared" si="0"/>
         <v>4300</v>

</xml_diff>

<commit_message>
Revert fRad equation to match PnET-II. Change layering algorithm so that cohorts within the same main layer do not have overlapping leaf area (side-by-side cylinders), and determining when cohorts separate into major layers is done by proportional differences in biomass, controlled by LayerThreshRatio parameter.  Eliminated MaxDevLyrAv parameter.
</commit_message>
<xml_diff>
--- a/deploy/docs/PnET-Succession function worksheet v4.0.xlsx
+++ b/deploy/docs/PnET-Succession function worksheet v4.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BRM\LANDIS_II\GitCode\Extension-PnET-Succession\deploy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7137A9C2-E7DC-4C0C-AF6C-6925F41B8192}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BFBC01-E2C4-49F3-AAEF-848EA069449D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PnET-Succ v. PnET-II" sheetId="9" r:id="rId1"/>
@@ -643,7 +643,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="313">
   <si>
     <t>Shape parameter</t>
   </si>
@@ -1583,6 +1583,15 @@
   </si>
   <si>
     <t>Compare two fRad curves with different HalfSat values</t>
+  </si>
+  <si>
+    <t>saturation</t>
+  </si>
+  <si>
+    <t>field capacity</t>
+  </si>
+  <si>
+    <t>wilting point</t>
   </si>
 </sst>
 </file>
@@ -46925,7 +46934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16:K23"/>
     </sheetView>
   </sheetViews>
@@ -47442,8 +47451,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:H20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -47953,12 +47962,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F22" t="s">
+        <v>310</v>
+      </c>
       <c r="G22">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <f>(1-(G22-$F$2)/($G$2-$F$2))</f>
-        <v>0.23809523809523814</v>
+        <f>IF(G22&lt;=$D$2,0,IF(G22&lt;=$E$2,(1-($E$2-G22)/($E$2-$D$2)),IF(G22&gt;=$G$2,0,IF(G22&gt;=$F$2,(1-(G22-$F$2)/($G$2-$F$2)),1))))</f>
+        <v>0</v>
       </c>
       <c r="L22" s="24">
         <f t="shared" si="3"/>
@@ -47978,6 +47990,16 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F23" t="s">
+        <v>311</v>
+      </c>
+      <c r="G23">
+        <v>3.37</v>
+      </c>
+      <c r="H23" s="24">
+        <f>IF(G23&lt;=$D$2,0,IF(G23&lt;=$E$2,(1-($E$2-G23)/($E$2-$D$2)),IF(G23&gt;=$G$2,0,IF(G23&gt;=$F$2,(1-(G23-$F$2)/($G$2-$F$2)),1))))</f>
+        <v>0.67400000000000004</v>
+      </c>
       <c r="L23" s="24">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -47995,6 +48017,16 @@
       <c r="B24" s="24">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>312</v>
+      </c>
+      <c r="G24">
+        <v>153</v>
+      </c>
+      <c r="H24" s="24">
+        <f>IF(G24&lt;=$D$2,0,IF(G24&lt;=$E$2,(1-($E$2-G24)/($E$2-$D$2)),IF(G24&gt;=$G$2,0,IF(G24&gt;=$F$2,(1-(G24-$F$2)/($G$2-$F$2)),1))))</f>
+        <v>0.16666666666666663</v>
       </c>
       <c r="L24" s="24">
         <f t="shared" si="3"/>

</xml_diff>